<commit_message>
Edited Design to modify to LDO regulator and improve board layout
</commit_message>
<xml_diff>
--- a/Hardware/board_100pin/assembly/F7_100pin_BOM.xlsx
+++ b/Hardware/board_100pin/assembly/F7_100pin_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffe636b6914998df/PhD/Phocoena-DAQ/Hardware/board_100pin/assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{3463CFE6-4F20-4279-B039-57C24179BBDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3E6D4B96-3C7E-4F6C-89F6-855D45113D3B}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{3463CFE6-4F20-4279-B039-57C24179BBDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BA3CB515-C191-49B1-AF97-C045E8EE30C0}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="18000" windowHeight="9397" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -765,7 +765,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,8 +908,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1092,6 +1110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1257,10 +1281,15 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1617,23 +1646,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="K51" sqref="K51:K52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.265625" customWidth="1"/>
-    <col min="8" max="8" width="31.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="118.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="118.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1659,7 +1688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1687,8 +1716,16 @@
       <c r="I2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J2">
+        <f>0.096</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="K2">
+        <f>J2*B2</f>
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1716,8 +1753,16 @@
       <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J3">
+        <f xml:space="preserve"> 0.0062</f>
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K48" si="0">J3*B3</f>
+        <v>2.4799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1745,8 +1790,16 @@
       <c r="I4" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J4">
+        <f>0.048</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1774,8 +1827,15 @@
       <c r="I5" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J5">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>8.5000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -1803,8 +1863,16 @@
       <c r="I6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J6">
+        <f xml:space="preserve"> 0.01914</f>
+        <v>1.9140000000000001E-2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>3.8280000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1829,8 +1897,16 @@
       <c r="H7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J7">
+        <f>0.10981</f>
+        <v>0.10981</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>0.32943</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1855,8 +1931,15 @@
       <c r="H8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J8">
+        <v>2.461E-2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>2.461E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -1881,11 +1964,18 @@
       <c r="H9" t="s">
         <v>47</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J9">
+        <v>0.1487</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>0.1487</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
@@ -1913,8 +2003,15 @@
       <c r="I10" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J10">
+        <v>0.12180000000000001</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>0.24360000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
@@ -1942,8 +2039,16 @@
       <c r="I11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J11">
+        <f xml:space="preserve"> 0.006 *B11</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -1971,8 +2076,15 @@
       <c r="I12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J12">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
@@ -2000,8 +2112,15 @@
       <c r="I13" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J13">
+        <v>5.5E-2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2029,8 +2148,15 @@
       <c r="I14" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J14">
+        <v>5.5E-2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>76</v>
       </c>
@@ -2058,8 +2184,15 @@
       <c r="I15" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J15">
+        <v>0.15029999999999999</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>0.15029999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>84</v>
       </c>
@@ -2087,8 +2220,15 @@
       <c r="I16" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J16" s="3">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>3.1399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>92</v>
       </c>
@@ -2116,8 +2256,15 @@
       <c r="I17" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J17" s="3">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>3.1399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>94</v>
       </c>
@@ -2136,8 +2283,12 @@
       <c r="F18" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>99</v>
       </c>
@@ -2156,8 +2307,12 @@
       <c r="F19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>101</v>
       </c>
@@ -2185,8 +2340,15 @@
       <c r="I20" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J20" s="3">
+        <v>3.9403999999999999</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>7.8807999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>108</v>
       </c>
@@ -2214,8 +2376,15 @@
       <c r="I21" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J21" s="4">
+        <v>0.92220000000000002</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>0.92220000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>114</v>
       </c>
@@ -2240,11 +2409,18 @@
       <c r="H22" t="s">
         <v>115</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J22" s="3">
+        <v>1.2979000000000001</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>1.2979000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>119</v>
       </c>
@@ -2272,8 +2448,15 @@
       <c r="I23" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J23" s="3">
+        <v>2.5417000000000001</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>2.5417000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>126</v>
       </c>
@@ -2292,8 +2475,12 @@
       <c r="F24" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>131</v>
       </c>
@@ -2312,8 +2499,12 @@
       <c r="F25" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>136</v>
       </c>
@@ -2332,8 +2523,12 @@
       <c r="F26" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>138</v>
       </c>
@@ -2352,8 +2547,12 @@
       <c r="F27" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>140</v>
       </c>
@@ -2372,8 +2571,12 @@
       <c r="F28" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>142</v>
       </c>
@@ -2395,8 +2598,15 @@
       <c r="I29" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J29" s="3">
+        <v>0.4017</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>0.4017</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>148</v>
       </c>
@@ -2424,8 +2634,15 @@
       <c r="I30" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J30" s="3">
+        <v>1.4645999999999999</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>1.4645999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>155</v>
       </c>
@@ -2450,8 +2667,15 @@
       <c r="H31" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J31" s="3">
+        <v>0.68908000000000003</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>1.3781600000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>161</v>
       </c>
@@ -2479,8 +2703,15 @@
       <c r="I32" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J32" s="3">
+        <v>0.1777</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>0.1777</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>169</v>
       </c>
@@ -2508,8 +2739,15 @@
       <c r="I33" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J33" s="3">
+        <v>9.1499999999999998E-2</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>9.1499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>173</v>
       </c>
@@ -2537,8 +2775,15 @@
       <c r="I34" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J34" s="3">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>3.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>178</v>
       </c>
@@ -2566,8 +2811,15 @@
       <c r="I35" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J35" s="4">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>4.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>182</v>
       </c>
@@ -2595,8 +2847,15 @@
       <c r="I36" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J36" s="3">
+        <v>8.14E-2</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>186</v>
       </c>
@@ -2624,8 +2883,15 @@
       <c r="I37" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J37" s="3">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>6.4600000000000005E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>190</v>
       </c>
@@ -2653,8 +2919,15 @@
       <c r="I38" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J38" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>193</v>
       </c>
@@ -2682,8 +2955,15 @@
       <c r="I39" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J39" s="3">
+        <v>8.14E-2</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>0.1628</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>197</v>
       </c>
@@ -2711,8 +2991,15 @@
       <c r="I40" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J40" s="3">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>1.38E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>202</v>
       </c>
@@ -2740,8 +3027,15 @@
       <c r="I41" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J41" s="3">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>8.3999999999999995E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>206</v>
       </c>
@@ -2769,8 +3063,15 @@
       <c r="I42" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J42" s="3">
+        <v>8.14E-2</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>0.40700000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>210</v>
       </c>
@@ -2798,8 +3099,15 @@
       <c r="I43" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J43" s="3">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="0"/>
+        <v>4.7399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>214</v>
       </c>
@@ -2827,8 +3135,15 @@
       <c r="I44" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J44" s="3">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="0"/>
+        <v>3.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>217</v>
       </c>
@@ -2856,8 +3171,15 @@
       <c r="I45" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J45" s="3">
+        <v>0.1227</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="0"/>
+        <v>0.1227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>223</v>
       </c>
@@ -2882,8 +3204,15 @@
       <c r="H46" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J46" s="3">
+        <v>1.29</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="0"/>
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>228</v>
       </c>
@@ -2911,8 +3240,15 @@
       <c r="I47" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J47" s="3">
+        <v>8.9096299999999999</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="0"/>
+        <v>8.9096299999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>235</v>
       </c>
@@ -2939,6 +3275,24 @@
       </c>
       <c r="I48" s="1" t="s">
         <v>242</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0.37569999999999998</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="0"/>
+        <v>0.37569999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <f>SUM(K2:K48)</f>
+        <v>29.577210000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <v>5.48</v>
       </c>
     </row>
   </sheetData>
@@ -2949,7 +3303,10 @@
     <hyperlink ref="I29" r:id="rId4" xr:uid="{2B4CC71F-F5B0-411E-8855-3105878C8434}"/>
     <hyperlink ref="I42" r:id="rId5" xr:uid="{49A717A1-A48D-4BD1-BA56-088997DD0423}"/>
     <hyperlink ref="I48" r:id="rId6" xr:uid="{47CE3408-D94F-4EDB-8686-51972DD14743}"/>
+    <hyperlink ref="I9" r:id="rId7" xr:uid="{6911D252-C2B6-4FC0-81F0-30EC6E7BD6AB}"/>
+    <hyperlink ref="I22" r:id="rId8" xr:uid="{7E249C4F-471D-473B-884D-7714E26C123C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>